<commit_message>
13 OCTOBER 2025 S417 system commit implement changes Time=15.30
</commit_message>
<xml_diff>
--- a/public/alumini_excel/phd_alumini.xlsx
+++ b/public/alumini_excel/phd_alumini.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\s417\dept_website\public\alumini_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0D31F1-1958-4C2F-82A5-B36D4BF37947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F17C803-192F-4212-BA24-5A040059D6C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AF22DF37-800A-494C-9687-3C55FE8C1945}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" xr2:uid="{AF22DF37-800A-494C-9687-3C55FE8C1945}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -224,7 +224,7 @@
     <t>Passed Out Year</t>
   </si>
   <si>
-    <t>PI/Guide</t>
+    <t>Guide</t>
   </si>
 </sst>
 </file>
@@ -599,7 +599,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>